<commit_message>
[Modified] : UseCase doc
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/Achievement/Achievement.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/Achievement/Achievement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\To-Do-App\ToDoApp-Doc\Document\Diagram\UseCase\Achievement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D1D839-95E7-4266-BBB6-A49F8A818211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEEE183-780E-4110-B7D1-D33309F8B90A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Record Achievement" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>Use-case number:</t>
   </si>
@@ -72,81 +72,22 @@
     <t>User</t>
   </si>
   <si>
-    <t>Người dùng chọn các chế độ xem khác</t>
-  </si>
-  <si>
     <t>Chức năng dùng để ghi lại thành tích mà người dùng đã vượt qua hoặc đạt được</t>
   </si>
   <si>
-    <t>_Người dùng vào More Option trong Achievement
-_Người dùng nhấn vào Manage Achievement
-_Người dùng chọn chế độ xem và nhấn vào từng thành phần để xem chi tiết các Achievement</t>
-  </si>
-  <si>
-    <t>_Lỗi mã nguồn
-_Nếu người dùng chưa hoàn thành các task thì sẽ không có các Achievement để hiển thị</t>
-  </si>
-  <si>
-    <t>Khi nhấn vào More Option sẽ hiển thị ra Manage Achievement</t>
-  </si>
-  <si>
-    <t>Người dùng phải đăng ký tài khoản trước đó</t>
-  </si>
-  <si>
     <t>Máy tính của người dùng ghi nhận thành công các Achievement và ở trạng thái sẵn sàng cho việc thực hiện một tác vụ khác</t>
   </si>
   <si>
-    <t xml:space="preserve">_Người dùng vào More Option trong Achievement
-_Người dùng nhấn vào Manage Achievement
-</t>
-  </si>
-  <si>
-    <t>Hệ thống lưu từng Achievement</t>
-  </si>
-  <si>
-    <t>Khi nhấn vào Manage Achievement phải hiển thị ra các chế độ xem</t>
-  </si>
-  <si>
     <t>Người dùng muốn xem các Achievement</t>
-  </si>
-  <si>
-    <t>Hệ thống sẽ hiển thị các Achievement ra màn hình và ở trạng thái sẵn sàng cho việc thực hiện 
-một tác vụ khác</t>
   </si>
   <si>
     <t>_Lỗi mã nguồn
 _Nếu không tồn tại Achievement nào thì thông báo cho người dùng biết</t>
   </si>
   <si>
-    <t>Người dùng phải hoàn thành ít nhất 1 task và máy của người dùng phải kết nối đến server</t>
-  </si>
-  <si>
     <t xml:space="preserve">Người dùng nhận được một số điểm tương ứng khi hoàn thành hoặc vượt qua một thử thách </t>
   </si>
   <si>
-    <t>_Người dùng vào More Option trong
-Achievement
-_Người dùng nhấn vào Manage Point để xem Point của mình
-_Hoặc có thể vào phần Settings trong Account để xem</t>
-  </si>
-  <si>
-    <t>Người dùng nhận Point bằng các hình thức khác không phải bằng việc hoàn thành task như share với bạn bè</t>
-  </si>
-  <si>
-    <t>_Lỗi mã nguồn
-_Nếu chưa có Point nào thì thông báo cho người dùng</t>
-  </si>
-  <si>
-    <t>Khi nhấn vào More Option sẽ hiển thị ra Manage Point</t>
-  </si>
-  <si>
-    <t>Người dùng hoàn thành xong một công việc nào đó</t>
-  </si>
-  <si>
-    <t>Người dùng phải hoàn thành ít nhất 1 công việc nào đó và máy của người dùng phải kết nối 
-đến server</t>
-  </si>
-  <si>
     <t>Máy tính của người dùng ghi nhận thành công Point và ở trạng thái sẵn sàng cho việc thực hiện một tác vụ khác</t>
   </si>
   <si>
@@ -162,51 +103,9 @@
     <t xml:space="preserve">Người dùng xem tất cả các Achievement </t>
   </si>
   <si>
-    <t xml:space="preserve">_Người dùng vào More Option trong
-Achievement
-_Hệ thống hiển thị danh mục các tùy chọn
-_Người dùng nhấn vào Manage Achievement
-_Hệ thống sẽ tự động ghi nhận các Achievement người dùng đạt được và lưu xuống database hoặc local storage
-</t>
-  </si>
-  <si>
-    <t>_Hệ thống hiển thị danh mục các tùy chọn
-_Hệ thống sẽ ghi nhận các Achievement đó và 
-lưu xuống database hoặc local storage</t>
-  </si>
-  <si>
     <t xml:space="preserve">Người dùng muốn đăng nhập vào ứng dụng và hoàn thành các task hoặc đạt đủ điều kiện của task </t>
   </si>
   <si>
-    <t>_Người dùng vào More Option trong
-Achievement
-_Hệ thống hiển thị danh mục các tùy chọn
-_Người dùng nhấn vào Manage Achievement
-_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
-_Người dùng chọn các chế độ xem để xem và nhấn vào từng cái để xem chi tiết ( như ngày, giờ,...)
-_Hệ thống sẽ hiển thị tất cả các Achievement của người dùng được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
-    <t>_Hệ thống hiển thị danh mục các tùy chọn
-_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
-_Sau đó sẽ hiển thị danh sách các Achievement ra màn hình được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
-    <t>_Hệ thống hiển thị danh mục các tùy chọn
-_Hệ thống sẽ tự động ghi nhận các Point của người dùng đạt được và cộng vào tài khoản người dùng
-_Hệ thống lưu dữ liệu xuống database hoặc local storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Người dùng vào More Option trong
-Achievement
-_Hệ thống hiển thị danh mục các tùy chọn
-_Người dùng nhấn vào Manage Point
-_Hệ thống sẽ tự động ghi nhận các Point của người dùng đạt được và cộng vào tài khoản người dùng
-_Người dùng nhấn vào để xem chi tiết hoặc có thể vào phần Settings trong Account để xem
-_Hệ thống lưu dữ liệu xuống database hoặc local storage
-</t>
-  </si>
-  <si>
     <t>Người dùng phải đạt được một số Achievement và khi nhấn vào More Option sẽ hiện ra mục Sharing</t>
   </si>
   <si>
@@ -225,7 +124,14 @@
     <t>Không có</t>
   </si>
   <si>
-    <t>_Người dùng nhấn vào icon Menu
+    <t xml:space="preserve">_Lỗi mã nguồn
+_Nếu chưa có bạn bè hoặc chưa liên kết các tài khoản khác như email, facebook,... thì thông báo cho người dùng </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người dùng phải hoàn thành ít nhất 1 công việc nào đó </t>
+  </si>
+  <si>
+    <t>_Người dùng nhấn vào Icon Menu
 _Hệ thống sẽ hiển thị ra Sidebar
 _Người dùng vào More Option ở phần Sidebar
 _Hệ thống hiển thị danh mục các tùy chọn
@@ -235,23 +141,110 @@
 _Hệ thống tải dữ liệu lên từ database hoặc local storage rồi rút gọn link và gửi link đó thông qua các chế độ chia sẻ mà người dùng đã chọn trước đó</t>
   </si>
   <si>
-    <t>__Người dùng nhấn vào icon Menu
+    <t>Khi nhấn vào More Option ( nằm phía trên bên phải trong Achievement) sẽ hiển thị ra Manage Point</t>
+  </si>
+  <si>
+    <t>Người dùng muốn nhận Point</t>
+  </si>
+  <si>
+    <t>Lỗi mã nguồn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+_Hệ thống sẽ tự động ghi nhận các Point của người dùng đạt được và cộng vào tài khoản người dùng
+_Hệ thống lưu dữ liệu xuống database hoặc local storage</t>
+  </si>
+  <si>
+    <t>Người dùng vào Account chọn phần Statistics rồi kéo xuống phần Achievement để xem</t>
+  </si>
+  <si>
+    <t>_Người dùng vào More Option trong Achievement
+_Người dùng nhấn vào Manage Achievement
+_Người dùng nhấn vào View Achievement
+_Người dùng chọn chế độ xem và nhấn vào từng thành phần để xem chi tiết các Achievement</t>
+  </si>
+  <si>
+    <t>Khi nhấn vào Manage Achievement phải hiển thị ra View Achievement để người dùng có thể lựa chọn</t>
+  </si>
+  <si>
+    <t>Người dùng phải hoàn thành ít nhất 1 task hoặc một nhiệm vụ cụ thể nào đó</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Người dùng hoàn thành một task hoặc nhiệm vụ nào đó
+_Hệ thống sẽ tự động ghi nhận các Point của người dùng đạt được và cộng vào tài khoản người dùng
+_Người dùng nhấn vào để xem chi tiết hoặc có thể vào phần Settings trong Account để xem
+_Hệ thống lưu dữ liệu xuống database hoặc local storage
+</t>
+  </si>
+  <si>
+    <t>_Người dùng hoàn thành một task hoặc nhiệm vụ của mình
+_Hoặc có thể vào phần Settings trong Account để xem</t>
+  </si>
+  <si>
+    <t>_Người dùng hoàn thành một task hoặc nhiệm vụ nào đó
+_Hệ thống sẽ tự động ghi nhận các Achievement của người dùng đạt được và thêm vào tài khoản người dùng
+_Người dùng nhấn vào để xem chi tiết hoặc có thể vào phần Settings trong Account để xem
+_Hệ thống lưu dữ liệu xuống database hoặc local storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Người dùng hoàn thành một task hoặc nhiệm vụ nào đó
+_Người dùng nhấn vào để xem chi tiết hoặc có thể vào phần Settings trong Account để xem
+</t>
+  </si>
+  <si>
+    <t>_Hệ thống sẽ tự động ghi nhận các Achievement của người dùng đạt được và thêm vào tài khoản người dùng
+_Hệ thống lưu dữ liệu xuống database hoặc local storage</t>
+  </si>
+  <si>
+    <t>_Lỗi mã nguồn
+_Nếu người dùng chưa hoàn thành các task hoặc nhiệm vụ thì sẽ không có các Achievement để hiển thị</t>
+  </si>
+  <si>
+    <t>Khi nhấn vào More Option ( nằm phía trên bên phải trong Achievement)  sẽ hiển thị ra Manage Achievement</t>
+  </si>
+  <si>
+    <t>Người dùng phải đăng ký tài khoản trước đó và hoàn thành những task hoặc nhiệm vụ có sẵn trên app</t>
+  </si>
+  <si>
+    <t>_Hệ thống hiển thị danh mục các tùy chọn
+_Hệ thống hiển thị các chế độ để lựa chọn
+_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
+_Sau đó hệ thống đánh dấu chế độ đã chọn và sẽ hiển thị danh sách các Achievement ra màn hình được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>_Người dùng nhấn vào Icon Menu
+_Hệ thống sẽ hiển thị ra Sidebar
+_Người dùng vào More Option ở phần Sidebar
+_Hệ thống hiển thị danh mục các tùy chọn
+_Người dùng nhấn vào mục Sharing
+_Hệ thống sẽ hiển thị ra hộp thoại để người dùng lựa chọn
+_Sau đó người dùng chọn các chế độ chia sẻ khác nhau ( như qua Email, Messenger, Facebook,...) và nhấn vào nút share để chia sẻ chúng
+_Hệ thống đánh dấu chế độ đã chọn và tải dữ liệu lên từ database hoặc local storage rồi rút gọn link và gửi link đó thông qua các chế độ chia sẻ mà người dùng đã chọn trước đó</t>
+  </si>
+  <si>
+    <t>_Hệ thống sẽ hiển thị ra Sidebar
+_Hệ thống hiển thị danh mục các tùy chọn
+_Hệ thống sẽ hiển thị ra hộp thoại hiển thị các chế độ chia sẻ để người dùng lựa chọn
+_Hệ thống đánh dấu chế độ đã chọn và tải dữ liệu lên từ database hoặc local storage rồi rút gọn link và gửi link đó thông qua các chế độ chia sẻ mà người dùng đã chọn trước đó</t>
+  </si>
+  <si>
+    <t>_Người dùng nhấn vào icon Menu
 _Người dùng vào More Option ở phần Slidebar
 _Người dùng nhấn vào mục Sharing
 _Người dùng chọn các chế độ chia sẻ khác nhau ( như qua Email, Messenger, Facebook,...) và nhấn vào nút share để chia sẻ chúng</t>
   </si>
   <si>
-    <t>_Hệ thống sẽ hiển thị ra Sidebar
+    <t>_Người dùng vào More Option trong Achievement
 _Hệ thống hiển thị danh mục các tùy chọn
-_Hệ thống sẽ hiển thị ra hộp thoại hiển thị các chế độ chia sẻ để người dùng lựa chọn
-_Hệ thống tải dữ liệu lên từ database hoặc local storage rồi rút gọn link và gửi link đó thông qua các chế độ chia sẻ mà người dùng đã chọn trước đó</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Lỗi mã nguồn
-_Nếu chưa có bạn bè hoặc chưa liên kết các tài khoản khác như email, facebook,... thì thông báo cho người dùng </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Người dùng phải hoàn thành ít nhất 1 công việc nào đó </t>
+_Người dùng nhấn vào Manage Achievement
+_Hệ thống hiển thị các chế độ để lựa chọn
+_Người dùng nhấn vào View Achievement
+_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
+_Người dùng chọn các chế độ xem để xem và nhấn vào từng cái để xem chi tiết ( như ngày, giờ,...)
+_Hệ thống đánh dấu chế độ đã chọn và sẽ hiển thị tất cả các Achievement của người dùng được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>Hệ thống sẽ hiển thị các Achievement ra màn hình và ở trạng thái sẵn sàng cho việc thực hiện một tác vụ khác</t>
   </si>
 </sst>
 </file>
@@ -649,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -678,7 +671,7 @@
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
@@ -687,10 +680,10 @@
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -699,21 +692,21 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -721,7 +714,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -730,7 +723,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E10" s="6"/>
     </row>
@@ -739,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="E11" s="6"/>
     </row>
@@ -748,7 +741,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E12" s="6"/>
     </row>
@@ -757,7 +750,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="E13" s="6"/>
     </row>
@@ -766,7 +759,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -792,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -821,7 +814,7 @@
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
@@ -830,10 +823,10 @@
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -842,21 +835,21 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="198" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" ht="159.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -864,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -873,7 +866,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E10" s="6"/>
     </row>
@@ -882,7 +875,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E11" s="6"/>
     </row>
@@ -891,7 +884,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E12" s="6"/>
     </row>
@@ -900,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="E13" s="6"/>
     </row>
@@ -909,7 +902,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -934,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -963,7 +956,7 @@
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
@@ -972,10 +965,10 @@
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -984,47 +977,47 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="6"/>
     </row>
@@ -1033,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E12" s="6"/>
     </row>
@@ -1042,7 +1035,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" s="6"/>
     </row>
@@ -1051,7 +1044,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -1076,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1105,7 +1098,7 @@
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
@@ -1114,10 +1107,10 @@
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -1126,21 +1119,21 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="198.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" ht="159" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1148,7 +1141,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -1157,7 +1150,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E10" s="6"/>
     </row>
@@ -1166,7 +1159,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E11" s="6"/>
     </row>
@@ -1175,7 +1168,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E12" s="6"/>
     </row>
@@ -1184,7 +1177,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E13" s="6"/>
     </row>
@@ -1193,7 +1186,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E14" s="6"/>
     </row>

</xml_diff>

<commit_message>
[Modified] : Achievement Rename
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/Achievement/Achievement.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/Achievement/Achievement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\To-Do-App\ToDoApp-Doc\Document\Diagram\UseCase\Achievement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEEE183-780E-4110-B7D1-D33309F8B90A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004CDADD-31C2-45C1-9D40-5DF5A3D394DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Record Achievement" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Use-case name:</t>
   </si>
   <si>
-    <t>Basle course of events:</t>
-  </si>
-  <si>
     <t>Alternative paths:</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>Hệ thống sẽ hiển thị các Achievement ra màn hình và ở trạng thái sẵn sàng cho việc thực hiện một tác vụ khác</t>
+  </si>
+  <si>
+    <t>Basic course of events:</t>
   </si>
 </sst>
 </file>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -665,101 +665,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -786,7 +786,7 @@
   <dimension ref="C3:E14"/>
   <sheetViews>
     <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:E14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -808,101 +808,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -927,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E11"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -950,101 +950,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="3:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1092,101 +1092,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="198.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="6"/>
     </row>

</xml_diff>